<commit_message>
.gitignore changed to not commit target folder content controller changes applied
</commit_message>
<xml_diff>
--- a/.timesheet/TimeSheet.xlsx
+++ b/.timesheet/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>1399/05/04</t>
   </si>
@@ -198,6 +198,33 @@
   </si>
   <si>
     <t>1399/06/21</t>
+  </si>
+  <si>
+    <t>1399/06/22</t>
+  </si>
+  <si>
+    <t>1399/06/23</t>
+  </si>
+  <si>
+    <t>1399/06/24</t>
+  </si>
+  <si>
+    <t>1399/06/25</t>
+  </si>
+  <si>
+    <t>1399/06/26</t>
+  </si>
+  <si>
+    <t>1399/06/27</t>
+  </si>
+  <si>
+    <t>1399/06/28</t>
+  </si>
+  <si>
+    <t>1399/06/29</t>
+  </si>
+  <si>
+    <t>1399/06/30</t>
   </si>
 </sst>
 </file>
@@ -233,12 +260,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,16 +547,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1159,6 +1188,12 @@
       <c r="B47" t="s">
         <v>55</v>
       </c>
+      <c r="C47" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1167,13 +1202,145 @@
       <c r="B48" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.70833333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>